<commit_message>
update: 更新 mybatis 基础笔记
</commit_message>
<xml_diff>
--- a/resources/attachments/MyBatis/01-MyBatis基础笔记-相关表格.xlsx
+++ b/resources/attachments/MyBatis/01-MyBatis基础笔记-相关表格.xlsx
@@ -1,23 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE94F1A-63CC-48E7-8341-7D77FF686516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="映射文件(Mapper.xml)主要配置总结" sheetId="1" r:id="rId1"/>
     <sheet name="SqlMapConfig.xml主要配置" sheetId="7" r:id="rId2"/>
     <sheet name="MyBatis支持的别名" sheetId="8" r:id="rId3"/>
     <sheet name="动态 SQL 主要标签" sheetId="9" r:id="rId4"/>
+    <sheet name="映射器注解" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="202">
   <si>
     <t>------------</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -530,14 +545,3120 @@
   </si>
   <si>
     <t>`&lt;choose&gt;`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注解</t>
+  </si>
+  <si>
+    <t>使用对象</t>
+  </si>
+  <si>
+    <t>XML 等价形式</t>
+  </si>
+  <si>
+    <t>类</t>
+  </si>
+  <si>
+    <t>&lt;cache&gt;</t>
+  </si>
+  <si>
+    <t>@Property</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>&lt;property&gt;</t>
+  </si>
+  <si>
+    <t>@CacheNamespaceRef</t>
+  </si>
+  <si>
+    <t>&lt;cacheRef&gt;</t>
+  </si>
+  <si>
+    <t>@ConstructorArgs</t>
+  </si>
+  <si>
+    <t>方法</t>
+  </si>
+  <si>
+    <t>&lt;constructor&gt;</t>
+  </si>
+  <si>
+    <t>@Arg</t>
+  </si>
+  <si>
+    <t>@TypeDiscriminator</t>
+  </si>
+  <si>
+    <t>&lt;discriminator&gt;</t>
+  </si>
+  <si>
+    <t>@Case</t>
+  </si>
+  <si>
+    <t>&lt;case&gt;</t>
+  </si>
+  <si>
+    <t>@Results</t>
+  </si>
+  <si>
+    <t>&lt;resultMap&gt;</t>
+  </si>
+  <si>
+    <t>@Result</t>
+  </si>
+  <si>
+    <t>@One</t>
+  </si>
+  <si>
+    <t>&lt;association&gt;</t>
+  </si>
+  <si>
+    <t>@Many</t>
+  </si>
+  <si>
+    <t>&lt;collection&gt;</t>
+  </si>
+  <si>
+    <t>@MapKey</t>
+  </si>
+  <si>
+    <t>@Options</t>
+  </si>
+  <si>
+    <t>映射语句的属性</t>
+  </si>
+  <si>
+    <t>&lt;insert&gt;
+&lt;update&gt;
+&lt;delete&gt;
+&lt;select&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Param</t>
+  </si>
+  <si>
+    <t>参数</t>
+  </si>
+  <si>
+    <t>@SelectKey</t>
+  </si>
+  <si>
+    <t>&lt;selectKey&gt;</t>
+  </si>
+  <si>
+    <t>@ResultMap</t>
+  </si>
+  <si>
+    <t>@ResultType</t>
+  </si>
+  <si>
+    <t>@Flush</t>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>为给定的命名空间（比如类）配置缓存。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>implemetation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>eviction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>flushInterval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>readWrite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>blocking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>properties</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">指定参数值或占位符（placeholder）（该占位符能被 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>mybatis-config.xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 内的配置属性替换）。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>。（仅在 MyBatis 3.4.2 以上可用）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>引用另外一个命名空间的缓存以供使用。注意，即使共享相同的全限定类名，在 XML 映射文件中声明的缓存仍被识别为一个独立的命名空间。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。如果你使用了这个注解，你应设置 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或者 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的其中一个。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性用于指定能够表示该命名空间的 Java 类型（命名空间名就是该 Java 类型的全限定类名），</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性（这个属性仅在 MyBatis 3.4.2 以上可用）则直接指定了命名空间的名字。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>收集一组结果以传递给一个结果对象的构造方法。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，它是一个 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Arg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 数组。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ConstructorArgs 集合的一部分，代表一个构造方法参数。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>javaType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>jdbcType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>typeHandler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>resultMap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。id 属性和 XML 元素 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;idArg&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 相似，它是一个布尔值，表示该属性是否用于唯一标识和比较对象。从版本 3.5.4 开始，该注解变为可重复注解。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>决定使用何种结果映射的一组取值（case）。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>javaType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>jdbcType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>typeHandler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。cases 属性是一个 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Case</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 的数组。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>表示某个值的一个取值以及该取值对应的映射。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。results 属性是一个 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 的数组，因此这个注解实际上和 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>ResultMap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 很相似，由下面的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解指定。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>一组结果映射，指定了对某个特定结果列，映射到某个属性或字段的方式。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。value 属性是一个 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解的数组。而 id 属性则是结果映射的名称。从版本 3.5.4 开始，该注解变为可重复注解。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>在列和属性或字段之间的单个结果映射。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>javaType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>jdbcType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>typeHandler</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>many</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。id 属性和 XML 元素 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;id&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 相似，它是一个布尔值，表示该属性是否用于唯一标识和比较对象。one 属性是一个关联，和 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;association&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 类似，而 many 属性则是集合关联，和 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;collection&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 类似。这样命名是为了避免产生名称冲突。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">复杂类型的单个属性映射。属性： </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，指定可加载合适类型实例的映射语句（也就是映射器方法）全限定名； </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>fetchType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，指定在该映射中覆盖全局配置参数 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>lazyLoadingEnabled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">； </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>resultMap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用）, 结果集的完全限定名，该结果映射到查询结果中的集合对象； </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>columnPrefix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用），在嵌套的结果集中对所查询的列进行分组的列前缀。 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>提示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解 API 不支持联合映射。这是由于 Java 注解不允许产生循环引用。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">复杂类型的集合属性映射。属性： </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，指定可加载合适类型实例集合的映射语句（也就是映射器方法）全限定名； </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>fetchType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，指定在该映射中覆盖全局配置参数 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>lazyLoadingEnabled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ； </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>resultMap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用），结果集的完全限定名，该结果映射到查询结果中的集合对象； </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>columnPrefix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用），在嵌套的结果集中对所查询的列进行分组的列前缀。 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>提示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解 API 不支持联合映射。这是由于 Java 注解不允许产生循环引用。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>供返回值为 Map 的方法使用的注解。它使用对象的某个属性作为 key，将对象 List 转化为 Map。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>，指定作为 Map 的 key 值的对象属性名。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>该注解允许你指定大部分开关和配置选项，它们通常在映射语句上作为属性出现。与在注解上提供大量的属性相比，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Options</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解提供了一致、清晰的方式来指定选项。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>useCache=true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>flushCache=FlushCachePolicy.DEFAULT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>resultSetType=DEFAULT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>statementType=PREPARED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>fetchSize=-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>timeout=-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>useGeneratedKeys=false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyProperty=""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyColumn=""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>resultSets=""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId=""</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。注意，Java 注解无法指定 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 值。因此，一旦你使用了 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Options</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解，你的语句就会被上述属性的默认值所影响。要注意避免默认值带来的非预期行为。 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用）, 如果有一个配置好的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>DatabaseIdProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, MyBatis 会加载不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性和带有匹配当前数据库 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的所有语句。如果同时存在带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 和不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的相同语句，则后者会被舍弃。 注意：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyColumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性只在某些数据库中有效（如 Oracle、PostgreSQL 等）。要了解更多关于 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyColumn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 和 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyProperty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 可选值信息，请查看“insert, update 和 delete”一节。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>每个注解分别代表将会被执行的 SQL 语句。它们用字符串数组（或单个字符串）作为参数。如果传递的是字符串数组，字符串数组会被连接成单个完整的字符串，每个字符串之间加入一个空格。这有效地避免了用 Java 代码构建 SQL 语句时产生的“丢失空格”问题。当然，你也可以提前手动连接好字符串。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，指定用来组成单个 SQL 语句的字符串数组。 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用）, 如果有一个配置好的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>DatabaseIdProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, MyBatis 会加载不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性和带有匹配当前数据库 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的所有语句。如果同时存在带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 和不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的相同语句，则后者会被舍弃。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">允许构建动态 SQL。这些备选的 SQL 注解允许你指定返回 SQL 语句的类和方法，以供运行时执行。（从 MyBatis 3.4.6 开始，可以使用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>CharSequence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 代替 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 来作为返回类型）。当执行映射语句时，MyBatis 会实例化注解指定的类，并调用注解指定的方法。你可以通过 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>ProviderContext</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 传递映射方法接收到的参数、"Mapper interface type" 和 "Mapper method"（仅在 MyBatis 3.4.5 以上支持）作为参数。（MyBatis 3.4 以上支持传入多个参数） 属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性用于指定类名 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性是 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 的别名, 你必须指定任意一个。 但是你如果在全局配置中指定 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>defaultSqlProviderType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ，两个属性都可以忽略)。 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 用于指定该类的方法名（从版本 3.5.1 开始，可以省略 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性，MyBatis 将会使用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>ProviderMethodResolver</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 接口解析方法的具体实现。如果解析失败，MyBatis 将会使用名为 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>provideSql</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 的降级实现）。</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>提示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 接下来的“SQL 语句构建器”一章将会讨论该话题，以帮助你以更清晰、更便于阅读的方式构建动态 SQL。 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用）, 如果有一个配置好的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>DatabaseIdProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, MyBatis 会加载不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性和带有匹配当前数据库 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的所有语句。如果同时存在带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 和不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的相同语句，则后者会被舍弃。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">如果你的映射方法接受多个参数，就可以使用这个注解自定义每个参数的名字。否则在默认情况下，除 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>RowBounds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 以外的参数会以 "param" 加参数位置被命名。例如 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>#{param1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>#{param2}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。如果使用了 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Param("person")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，参数就会被命名为 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>#{person}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">这个注解的功能与 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;selectKey&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 标签完全一致。该注解只能在 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Insert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@InsertProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@UpdateProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 标注的方法上使用，否则将会被忽略。如果标注了 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@SelectKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解，MyBatis 将会忽略掉由 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Options</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解所设置的生成主键或设置（configuration）属性。属性：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>statement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 以字符串数组形式指定将会被执行的 SQL 语句，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyProperty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 指定作为参数传入的对象对应属性的名称，该属性将会更新成新的值，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>before</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 可以指定为 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 以指明 SQL 语句应被在插入语句的之前还是之后执行。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>resultType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 则指定 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>keyProperty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 的 Java 类型。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>statementType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 则用于选择语句类型，可以选择 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>STATEMENT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>PREPARED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>CALLABLE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 之一，它们分别对应于 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>Statement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>PreparedStatement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 和 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>CallableStatement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。默认值是 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>PREPARED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">。 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（3.5.5以上可用）, 如果有一个配置好的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>DatabaseIdProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, MyBatis 会加载不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性和带有匹配当前数据库 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的所有语句。如果同时存在带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 和不带 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>databaseId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 属性的相同语句，则后者会被舍弃。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">这个注解为 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或者 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@SelectProvider</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解指定 XML 映射中 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;resultMap&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 元素的 id。这使得注解的 select 可以复用已在 XML 中定义的 ResultMap。如果标注的 select 注解中存在 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@Results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 或者 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@ConstructorArgs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解，这两个注解将被此注解覆盖。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">在使用了结果处理器的情况下，需要使用此注解。由于此时的返回类型为 void，所以 Mybatis 需要有一种方法来判断每一行返回的对象类型。如果在 XML 有对应的结果映射，请使用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>@ResultMap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 注解。如果结果类型在 XML 的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;select&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 元素中指定了，就不需要使用其它注解了。否则就需要使用此注解。比如，如果一个标注了 @Select 的方法想要使用结果处理器，那么它的返回类型必须是 void，并且必须使用这个注解（或者 @ResultMap）。这个注解仅在方法返回类型是 void 的情况下生效。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">如果使用了这个注解，定义在 Mapper 接口中的方法就能够调用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFFF3502"/>
+        <rFont val="Source Code Pro"/>
+        <family val="3"/>
+      </rPr>
+      <t>SqlSession#flushStatements()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Vollkorn"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 方法。（Mybatis 3.3 以上可用）</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;arg&gt;
+&lt;idArg&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;result&gt;
+&lt;id&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Insert
+@Update
+@Delete
+@Select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@InsertProvider
+@UpdateProvider
+@DeleteProvider
+@SelectProvider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@CacheNamespace</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +3686,61 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFFF3502"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Vollkorn"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Vollkorn"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Vollkorn"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Vollkorn"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -602,7 +3778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -623,6 +3799,30 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -709,7 +3909,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -784,6 +3984,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -819,6 +4036,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -994,14 +4228,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="1" customWidth="1"/>
@@ -1012,7 +4246,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:8">
       <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1020,7 +4254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +4272,7 @@
         <v>|标签名|相关属性|作用说明|父标签|</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +4290,7 @@
         <v>|------------|------------|------------|------------|</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" ht="27">
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1072,7 +4306,7 @@
         <v>|`&lt;mapper&gt;`|属性namespace：namespace命名空间，作用就是对sql进行分类化管理，理解为sql隔离&lt;br/&gt;注意：使用mapper代理方法开发，namespace有特殊重要的作用，直接指向mapper接口的类路径。|映射文件的根标签||</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="148.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" ht="148.5">
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1090,7 +4324,7 @@
         <v>|`&lt;select&gt;`|`id`：表示当前`&lt;select&gt;`标签的唯一标识（将sql语句封装到mappedStatement对象中，将id称为mappedStatement的id）&lt;br/&gt;`parameterType`：指定输入参数的类型，当参数传递的是集合或者数组的时候，在实际开发中建议都写list&lt;br/&gt;一般使用`#{}`实现的是向prepareStatement中的预处理语句中设置参数值（“`?`”占位符）&lt;br/&gt;`resultType`：指定查询返回结果的输出类型，如果返回的结果是一个实体类，&lt;font color=red&gt;必须要求实体类的属性和表的字段名称相同&lt;/font&gt;&lt;br/&gt;&lt;br/&gt;以下属性了解：&lt;br/&gt;resultMap：也是一个输出类型，配合&lt;resultMap&gt;标签使用&lt;br/&gt;flushCache：设置查询的时候是否清空缓存，默认为false&lt;br/&gt;useCache：将查询结果放入缓存中，默认为true&lt;br/&gt;timeout：设置查询返回结果的最大响应时间&lt;br/&gt;fetchSize：每次批量返回的结果行数。默认不设置&lt;br/&gt;statementType：STATEMENT、PREPARED或CALLABLE的一种，这会让MyBatis使用选择Statement、PreparedStatement或CallableStatement。默认值：PREPARED&lt;br/&gt;resultSetType：设置游标FORWARD_ONLY、SCROLL_SENSITIVE、SCROLL_INSENSITIVE中的一种。认不设置|用于编写查询语句用的标签|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" ht="27">
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1108,7 +4342,7 @@
         <v>|`&lt;insert&gt;`|id/parameterType属性一样|用于编写插入语句用的标签|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" ht="27">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1126,7 +4360,7 @@
         <v>|`&lt;update&gt;`|id/parameterType属性一样|用于编写更新语句用的标签|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" ht="27">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +4378,7 @@
         <v>|`&lt;delete&gt;`|id/parameterType属性一样|用于编写删除语句用的标签|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="40.5">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1162,7 +4396,7 @@
         <v>|`&lt;resultMap&gt;`|`type`属性：要映射的类型&lt;br/&gt;`id`属性：唯一标识，通过id引用该resultMap&lt;br/&gt;&lt;br/&gt;子标签`&lt;id&gt;`、子标签&lt;result&gt;配置订单的主键对应关系，其中属性`column`：主键字段（表），属性`property`：主键属性（pojo）|用于解决实体类中属性和表字段名不相同的问题|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" ht="40.5">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1178,7 +4412,7 @@
         <v>|`&lt;sql&gt;`||可以重用的SQL语句，可以被其他语句引用|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="54">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -1196,7 +4430,7 @@
         <v>|`&lt;selectKey&gt;`|`select LAST_INSERT_ID()`：得到刚刚insert操作添加的记录的主键，只适用与自增主键&lt;br/&gt;&lt;br/&gt;`keyColumn`属性：主键字段名（表）&lt;br/&gt;`keyProperty`属性：将查询到主键值设置到`parameterType`指定的对象的哪一个属性中&lt;br/&gt;`order`属性：指定`select LAST_INSERT_ID()`执行顺序，相对于insert语句来说的执行顺序&lt;br/&gt;`resultType`属性：指定`select LAST_INSERT_ID()`的结果类型|将插入数据的主键返回，返回到Customer对象中|`&lt;insert&gt;`|</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" ht="54">
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1212,7 +4446,7 @@
         <v>|`&lt;cache&gt;`||&lt;font color=red&gt;（不使用）&lt;/font&gt;配置给定命名空间缓存|`&lt;mapper&gt;`|</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" ht="67.5">
       <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
@@ -1236,14 +4470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" style="1" bestFit="1" customWidth="1"/>
@@ -1254,7 +4488,7 @@
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:7">
       <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1262,7 +4496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7">
       <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
@@ -1277,7 +4511,7 @@
         <v>|顺序|配置标签名称|说明|</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +4526,7 @@
         <v>|------------|------------|------------|</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7">
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
@@ -1307,7 +4541,7 @@
         <v>|1|properties|属性|</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7">
       <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
@@ -1322,7 +4556,7 @@
         <v>|2|settings|配置全局配置参数|</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7">
       <c r="B6" s="5" t="s">
         <v>38</v>
       </c>
@@ -1337,7 +4571,7 @@
         <v>|3|typeAliases|类型别名|</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:7">
       <c r="B7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1352,7 +4586,7 @@
         <v>|4|typeHandlers|类型处理器|</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:7">
       <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
@@ -1367,7 +4601,7 @@
         <v>|5|objectFactory|对象工厂|</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:7">
       <c r="B9" s="5" t="s">
         <v>41</v>
       </c>
@@ -1382,7 +4616,7 @@
         <v>|6|plugins|插件|</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:7">
       <c r="B10" s="5" t="s">
         <v>42</v>
       </c>
@@ -1397,7 +4631,7 @@
         <v>|7|environments|环境集合属性对象|</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:7">
       <c r="B11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1412,7 +4646,7 @@
         <v>|7-1|environment|环境子属性对象|</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:7">
       <c r="B12" s="5" t="s">
         <v>45</v>
       </c>
@@ -1427,7 +4661,7 @@
         <v>|7-1-1|transactionManager|事务管理|</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:7">
       <c r="B13" s="5" t="s">
         <v>46</v>
       </c>
@@ -1442,7 +4676,7 @@
         <v>|7-1-2|databaseIdProvider|多数据库支持|</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:7">
       <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
@@ -1465,14 +4699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="1" customWidth="1"/>
@@ -1483,7 +4717,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:8">
       <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1491,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8">
       <c r="B2" s="2" t="s">
         <v>72</v>
       </c>
@@ -1509,7 +4743,7 @@
         <v>|别名|映射类型|别名|映射类型|</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +4761,7 @@
         <v>|------------|------------|------------|------------|</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8">
       <c r="B4" s="5" t="s">
         <v>109</v>
       </c>
@@ -1545,7 +4779,7 @@
         <v>|`_byte`|byte|double|Double|</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8">
       <c r="B5" s="5" t="s">
         <v>110</v>
       </c>
@@ -1563,7 +4797,7 @@
         <v>|`_long`|long|float|Float|</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8">
       <c r="B6" s="5" t="s">
         <v>111</v>
       </c>
@@ -1581,7 +4815,7 @@
         <v>|`_short`|short|boolean|Boolean|</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8">
       <c r="B7" s="5" t="s">
         <v>112</v>
       </c>
@@ -1599,7 +4833,7 @@
         <v>|`_int`|int|date|Date|</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8">
       <c r="B8" s="5" t="s">
         <v>113</v>
       </c>
@@ -1617,7 +4851,7 @@
         <v>|`_integer`|int|decimal|BigDecimal|</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8">
       <c r="B9" s="5" t="s">
         <v>114</v>
       </c>
@@ -1635,7 +4869,7 @@
         <v>|`_double`|double|bigdecimal|BigDecimal|</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8">
       <c r="B10" s="5" t="s">
         <v>115</v>
       </c>
@@ -1653,7 +4887,7 @@
         <v>|`_float`|float|object|Object|</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8">
       <c r="B11" s="5" t="s">
         <v>116</v>
       </c>
@@ -1671,7 +4905,7 @@
         <v>|`_boolean`|boolean|map|Map|</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8">
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1689,7 +4923,7 @@
         <v>|string|String|hashmap|HashMap|</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8">
       <c r="B13" s="5" t="s">
         <v>76</v>
       </c>
@@ -1707,7 +4941,7 @@
         <v>|byte|Byte|list|List|</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8">
       <c r="B14" s="5" t="s">
         <v>79</v>
       </c>
@@ -1725,7 +4959,7 @@
         <v>|long|Long|arraylist|ArrayList|</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8">
       <c r="B15" s="5" t="s">
         <v>82</v>
       </c>
@@ -1743,7 +4977,7 @@
         <v>|short|Short|collection|Collection|</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:8">
       <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1761,7 +4995,7 @@
         <v>|int|Integer|iterator|Iterator|</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7">
       <c r="B17" s="5" t="s">
         <v>108</v>
       </c>
@@ -1783,14 +5017,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" style="1" bestFit="1" customWidth="1"/>
@@ -1801,7 +5035,7 @@
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:7">
       <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1809,7 +5043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7">
       <c r="B2" s="2" t="s">
         <v>118</v>
       </c>
@@ -1824,7 +5058,7 @@
         <v>|标签名|属性|说明|</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +5073,7 @@
         <v>|------------|------------|------------|</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15.75">
       <c r="B4" s="5" t="s">
         <v>122</v>
       </c>
@@ -1854,7 +5088,7 @@
         <v>|`&lt;if&gt;`|test：判断条件|根据条件判断拼接标签体的sql语句|</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7" ht="40.5">
       <c r="B5" s="5" t="s">
         <v>123</v>
       </c>
@@ -1867,7 +5101,7 @@
         <v>|`&lt;where&gt;`||1.where标签，相当于sql语句中的where关键字&lt;br/&gt;2.根据传入的参数情况，智能的去掉多余的and，or关键字&lt;br/&gt;3.根据传入的参数情况，智能的去掉多余的where关键字|</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7" ht="27">
       <c r="B6" s="5" t="s">
         <v>139</v>
       </c>
@@ -1882,7 +5116,7 @@
         <v>|`&lt;choose&gt;`|子标签：&lt;br/&gt;`&lt;when&gt;`、`&lt;otherwise&gt;`标签|相当于java中的switch，如果满足条件则不会再往下执行|</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:7" ht="27">
       <c r="B7" s="5" t="s">
         <v>124</v>
       </c>
@@ -1895,7 +5129,7 @@
         <v>|`&lt;set&gt;`||1.相当于sql语句中的set关键字&lt;br/&gt;2.根据传入的参数情况，智能的去掉最后一个多余的逗号|</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:7" ht="67.5">
       <c r="B8" s="5" t="s">
         <v>125</v>
       </c>
@@ -1910,7 +5144,7 @@
         <v>|`&lt;foreach&gt;`|`collection`：参数集合&lt;br/&gt;`item`：当前循环的对象引用&lt;br/&gt;`open`：拼装的sql语句片段开始&lt;br/&gt;`close`：拼装的sql语句片段的结束&lt;br/&gt;`separator`：指定元素之间的分割符|循环遍历处理参数集合（List、数组）|</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:7">
       <c r="B9" s="5" t="s">
         <v>126</v>
       </c>
@@ -1925,7 +5159,7 @@
         <v>|`&lt;sql&gt;`|id：唯一标识的名称，根据id引用该sql片段|提取公共的sql语句片段|</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:7">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -1940,7 +5174,7 @@
         <v>|`&lt;include&gt;`|refid：引用sql片段的id值|引用sql片段|</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:7">
       <c r="B11" s="5" t="s">
         <v>128</v>
       </c>
@@ -1951,6 +5185,323 @@
       <c r="F11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>|`&lt;trim&gt;`||格式化|</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD524C1-C015-4098-8C6C-AF621A8AC017}">
+  <dimension ref="B1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="1.875" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="108" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="9" customHeight="1"/>
+    <row r="2" spans="2:5" ht="20.100000000000001" customHeight="1">
+      <c r="B2" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="34.5">
+      <c r="B3" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="27">
+      <c r="B4" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="54">
+      <c r="B5" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="14.25">
+      <c r="B6" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="41.25">
+      <c r="B7" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="27">
+      <c r="B8" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="28.5">
+      <c r="B9" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="27">
+      <c r="B10" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="42.75">
+      <c r="B11" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="55.5">
+      <c r="B12" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="55.5">
+      <c r="B13" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="27">
+      <c r="B14" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="114">
+      <c r="B15" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="68.25">
+      <c r="B16" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="141">
+      <c r="B17" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="28.5">
+      <c r="B18" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="114">
+      <c r="B19" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="28.5">
+      <c r="B20" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="52.5">
+      <c r="B21" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="14.25">
+      <c r="B22" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>